<commit_message>
Minor fixes in group merges (#469)
* add support for grouped cells

* fix for rows after endgroup

* minor fix for text after grouping

* fix unit tests

* fix unit tests and docs

* minor fix

* Add support to vertical merge cells

* minor fixes in merge cells

* minor fix

* fix complex scenario

* finalize changes
</commit_message>
<xml_diff>
--- a/samples/xlsx/TestMergeSameCells.xlsx
+++ b/samples/xlsx/TestMergeSameCells.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developer\Eynar_Haji\MiniExcel\samples\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFC7F30-CB4D-41C4-854F-B12BDEDAD317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D09BA3-27B8-4911-B576-DE61710552EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5445" yWindow="4080" windowWidth="21600" windowHeight="11385" xr2:uid="{7E981748-3504-47EF-B8C2-B8AC12E673A0}"/>
+    <workbookView xWindow="8505" yWindow="5130" windowWidth="21600" windowHeight="11385" xr2:uid="{7E981748-3504-47EF-B8C2-B8AC12E673A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
   <si>
     <t>Department</t>
   </si>
@@ -58,6 +58,18 @@
   </si>
   <si>
     <t>Peter</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>05.02.2023</t>
+  </si>
+  <si>
+    <t>13.02.2023</t>
+  </si>
+  <si>
+    <t>15.02.2023</t>
   </si>
 </sst>
 </file>
@@ -108,21 +120,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,71 +452,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09AA2534-9DCC-48AE-B14E-CC9BD90C7542}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="C3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="D4" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="C6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>